<commit_message>
updated gui test file
</commit_message>
<xml_diff>
--- a/documentation/GUI-Test/gui_test_v0.1.xlsx
+++ b/documentation/GUI-Test/gui_test_v0.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz_Laptop\Desktop\sopro\gruppe03-team04\documentation\GUI-Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Desktop\SoproNEU\documentation\GUI-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12225A5A-0BE1-4C65-862A-E4D4AAC71B88}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE97AD4-A5F1-4D88-AC84-593E85C9E177}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,25 +224,13 @@
     <t>Csv  deutsch/English</t>
   </si>
   <si>
-    <t> (opt. Beschreibung noch mit rein)</t>
-  </si>
-  <si>
     <t>Word Deutsch</t>
   </si>
   <si>
-    <t> Query ID fehlt , Grafik sieht schrift bug</t>
-  </si>
-  <si>
     <t>Word englisch</t>
   </si>
   <si>
-    <t> Gleiche probleme wie beim Deutschen(+ keine Sprachunterscheidung)</t>
-  </si>
-  <si>
     <t>Pdf Deutsch/englisch</t>
-  </si>
-  <si>
-    <t> Crtical user name und access pattern id fehlt, + grafik schrift bug, IMMER NOCH!!!!!!</t>
   </si>
   <si>
     <t>Anaylse Durchführen</t>
@@ -270,22 +258,6 @@
     <t>Sap Settings aus liste auswählen</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> Man kann nicht die SAP- Verbindung vor der Konfiguration auswählen </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Beschreibung zur tabelle hinzufügen</t>
-    </r>
-  </si>
-  <si>
     <t>Combobox:</t>
   </si>
   <si>
@@ -293,21 +265,6 @@
   </si>
   <si>
     <t>SAP- Verbindung Combobox</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> (!Funktioniert) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Man kann nicht die SAP- Verbindung vor der Konfiguration auswählen</t>
-    </r>
   </si>
   <si>
     <t>Konfiguration aus Liste wählen</t>
@@ -687,9 +644,6 @@
     <t xml:space="preserve"> (+ zugehöriger Dialog) </t>
   </si>
   <si>
-    <t> Feedback wenn nicht alle eingaben gemacht wurden bzw. wenn das Pattern fehlt</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve"> Funktioniert </t>
     </r>
@@ -938,8 +892,73 @@
     <t>Verwendete Whitelist wirft wenn man sie verändert und speichern will eine Nullpointer Exception</t>
   </si>
   <si>
+    <t>Nutzermanagement:</t>
+  </si>
+  <si>
+    <t>In Zwischenablage Kopieren</t>
+  </si>
+  <si>
+    <t> Funktioniert ,</t>
+  </si>
+  <si>
+    <t>Checkboxen:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin </t>
+  </si>
+  <si>
+    <t>Datenanalyst</t>
+  </si>
+  <si>
+    <t>Viewer</t>
+  </si>
+  <si>
+    <t>Nutzername</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve"> Funktioniert </t>
+      <t> Funktioniert</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Man kann nicht die SAP- Verbindung vor der Konfiguration auswählen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Man kann nicht die SAP- Verbindung vor der Konfiguration auswählen</t>
     </r>
     <r>
       <rPr>
@@ -949,36 +968,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Fehler beim Speichern</t>
+      <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>Nutzermanagement:</t>
-  </si>
-  <si>
-    <t>In Zwischenablage Kopieren</t>
-  </si>
-  <si>
-    <t> Funktioniert ,</t>
-  </si>
-  <si>
-    <t>Checkboxen:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin </t>
-  </si>
-  <si>
-    <t>Datenanalyst</t>
-  </si>
-  <si>
-    <t>Viewer</t>
-  </si>
-  <si>
-    <t>Nutzername</t>
-  </si>
-  <si>
     <r>
-      <t> Funktioniert Opt.:</t>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Beschreibung zur tabelle hinzufügen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Funktioniert</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Query ID fehlt , Grafik sieht schrift bug</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Funktioniert</t>
     </r>
     <r>
       <rPr>
@@ -988,18 +1025,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gleiche probleme wie beim Deutschen(+ keine Sprachunterscheidung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>  Funktioniert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Crtical user name und access pattern id fehlt, + grafik schrift bug</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(opt. Beschreibung noch mit rein)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Funktioniert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feedback wenn nicht alle eingaben gemacht wurden bzw. wenn das Pattern fehlt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Funktioniert </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fehler beim Speichern</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> Funktioniert Opt.:</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Validierung nach Abbruch (beim Anlegen eines Neuen Nutzers)</t>
     </r>
-  </si>
-  <si>
-    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,6 +1386,12 @@
       <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1572,7 +1738,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1623,10 +1789,16 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1635,11 +1807,8 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -11336,8 +11505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="G215" sqref="G215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11454,36 +11623,36 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
@@ -11865,7 +12034,7 @@
         <v>50</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11875,10 +12044,10 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11888,10 +12057,10 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11901,10 +12070,10 @@
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11940,10 +12109,10 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11953,7 +12122,7 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>12</v>
@@ -11966,10 +12135,10 @@
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -11986,13 +12155,13 @@
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>12</v>
@@ -12005,10 +12174,10 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12024,7 +12193,7 @@
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="C51" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>9</v>
@@ -12047,7 +12216,7 @@
         <v>26</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12057,7 +12226,7 @@
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G53" s="12" t="s">
         <v>12</v>
@@ -12070,7 +12239,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G54" s="12" t="s">
         <v>12</v>
@@ -12087,7 +12256,7 @@
         <v>10</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>12</v>
@@ -12107,14 +12276,14 @@
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12124,29 +12293,29 @@
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="7"/>
       <c r="C59" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12156,10 +12325,10 @@
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12180,13 +12349,13 @@
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G62" s="12" t="s">
         <v>12</v>
@@ -12203,10 +12372,10 @@
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="5" t="s">
@@ -12227,10 +12396,10 @@
       <c r="D65" s="5"/>
       <c r="E65" s="10"/>
       <c r="F65" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12240,7 +12409,7 @@
       <c r="D66" s="5"/>
       <c r="E66" s="10"/>
       <c r="F66" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G66" s="12" t="s">
         <v>12</v>
@@ -12253,7 +12422,7 @@
       <c r="D67" s="5"/>
       <c r="E67" s="10"/>
       <c r="F67" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G67" s="12" t="s">
         <v>12</v>
@@ -12266,7 +12435,7 @@
       <c r="D68" s="5"/>
       <c r="E68" s="10"/>
       <c r="F68" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>12</v>
@@ -12299,7 +12468,7 @@
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G71" s="12" t="s">
         <v>12</v>
@@ -12312,10 +12481,10 @@
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12334,7 +12503,7 @@
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G74" s="12" t="s">
         <v>12</v>
@@ -12386,7 +12555,7 @@
         <v>10</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>12</v>
@@ -12405,16 +12574,16 @@
       <c r="A80" s="13"/>
       <c r="B80" s="7"/>
       <c r="C80" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>12</v>
@@ -12427,7 +12596,7 @@
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="11" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>12</v>
@@ -12440,7 +12609,7 @@
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="11" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G82" s="12" t="s">
         <v>12</v>
@@ -12453,7 +12622,7 @@
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>12</v>
@@ -12466,7 +12635,7 @@
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="F84" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>12</v>
@@ -12479,10 +12648,10 @@
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12505,7 +12674,7 @@
         <v>10</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G87" s="12" t="s">
         <v>12</v>
@@ -12518,7 +12687,7 @@
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>12</v>
@@ -12548,10 +12717,10 @@
     </row>
     <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="10" t="s">
@@ -12572,7 +12741,7 @@
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
       <c r="F92" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>12</v>
@@ -12585,10 +12754,10 @@
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
       <c r="F93" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G93" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12598,7 +12767,7 @@
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
       <c r="F94" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>12</v>
@@ -12611,7 +12780,7 @@
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
       <c r="F95" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>12</v>
@@ -12644,7 +12813,7 @@
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
       <c r="F98" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>12</v>
@@ -12657,10 +12826,10 @@
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G99" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12670,7 +12839,7 @@
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G100" s="12" t="s">
         <v>12</v>
@@ -12699,7 +12868,7 @@
         <v>35</v>
       </c>
       <c r="G102" s="12" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12722,7 +12891,7 @@
         <v>10</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>12</v>
@@ -12741,7 +12910,7 @@
       <c r="A106" s="13"/>
       <c r="B106" s="2"/>
       <c r="C106" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>9</v>
@@ -12755,29 +12924,29 @@
       <c r="G106" s="14"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="19"/>
-      <c r="B107" s="23"/>
-      <c r="C107" s="23"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="22"/>
+      <c r="A107" s="20"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
       <c r="F107" s="11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G107" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="19"/>
-      <c r="B108" s="23"/>
-      <c r="C108" s="23"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="22"/>
+      <c r="A108" s="20"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
       <c r="F108" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12787,35 +12956,35 @@
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
       <c r="F109" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G109" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="19"/>
-      <c r="B110" s="23"/>
-      <c r="C110" s="23"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="22"/>
+      <c r="A110" s="20"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
       <c r="F110" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G110" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G110" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="19"/>
-      <c r="B111" s="23"/>
-      <c r="C111" s="23"/>
-      <c r="D111" s="22"/>
-      <c r="E111" s="22"/>
+      <c r="A111" s="20"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
       <c r="F111" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G111" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="G111" s="19"/>
     </row>
     <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
@@ -12824,10 +12993,10 @@
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
       <c r="F112" s="11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G112" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12837,7 +13006,7 @@
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
       <c r="F113" s="11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G113" s="12" t="s">
         <v>12</v>
@@ -12850,10 +13019,10 @@
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
       <c r="F114" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G114" s="15" t="s">
-        <v>114</v>
+        <v>94</v>
+      </c>
+      <c r="G114" s="24" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12883,13 +13052,13 @@
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G117" s="12" t="s">
         <v>12</v>
@@ -12902,7 +13071,7 @@
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
       <c r="F118" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G118" s="12" t="s">
         <v>12</v>
@@ -12922,16 +13091,16 @@
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G120" s="12" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12941,10 +13110,10 @@
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
       <c r="F121" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G121" s="12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -12967,7 +13136,7 @@
         <v>34</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G123" s="12" t="s">
         <v>12</v>
@@ -12986,7 +13155,7 @@
       <c r="A125" s="13"/>
       <c r="B125" s="2"/>
       <c r="C125" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>9</v>
@@ -13000,29 +13169,29 @@
       <c r="G125" s="14"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="19"/>
-      <c r="B126" s="23"/>
-      <c r="C126" s="23"/>
-      <c r="D126" s="22"/>
-      <c r="E126" s="22"/>
+      <c r="A126" s="20"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="18"/>
       <c r="F126" s="11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G126" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="19"/>
-      <c r="B127" s="23"/>
-      <c r="C127" s="23"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="22"/>
+      <c r="A127" s="20"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="18"/>
+      <c r="E127" s="18"/>
       <c r="F127" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G127" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13032,35 +13201,35 @@
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
       <c r="F128" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G128" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="19"/>
-      <c r="B129" s="23"/>
-      <c r="C129" s="23"/>
-      <c r="D129" s="22"/>
-      <c r="E129" s="22"/>
+      <c r="A129" s="20"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="18"/>
+      <c r="E129" s="18"/>
       <c r="F129" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G129" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G129" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="19"/>
-      <c r="B130" s="23"/>
-      <c r="C130" s="23"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="22"/>
+      <c r="A130" s="20"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
       <c r="F130" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G130" s="18"/>
+        <v>118</v>
+      </c>
+      <c r="G130" s="19"/>
     </row>
     <row r="131" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
@@ -13069,10 +13238,10 @@
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
       <c r="F131" s="11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G131" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13082,7 +13251,7 @@
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
       <c r="F132" s="11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G132" s="12" t="s">
         <v>12</v>
@@ -13095,10 +13264,10 @@
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
       <c r="F133" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G133" s="15" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13128,13 +13297,13 @@
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G136" s="12" t="s">
         <v>12</v>
@@ -13147,7 +13316,7 @@
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
       <c r="F137" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>12</v>
@@ -13167,16 +13336,16 @@
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G139" s="12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13186,10 +13355,10 @@
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
       <c r="F140" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G140" s="12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13212,7 +13381,7 @@
         <v>34</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G142" s="12" t="s">
         <v>12</v>
@@ -13229,10 +13398,10 @@
     </row>
     <row r="144" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C144" s="7"/>
       <c r="D144" s="10" t="s">
@@ -13253,7 +13422,7 @@
       <c r="D145" s="10"/>
       <c r="E145" s="10"/>
       <c r="F145" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G145" s="12" t="s">
         <v>12</v>
@@ -13266,7 +13435,7 @@
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
       <c r="F146" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G146" s="12" t="s">
         <v>12</v>
@@ -13279,7 +13448,7 @@
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
       <c r="F147" s="11" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G147" s="12" t="s">
         <v>12</v>
@@ -13292,7 +13461,7 @@
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
       <c r="F148" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G148" s="12" t="s">
         <v>12</v>
@@ -13305,7 +13474,7 @@
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
       <c r="F149" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G149" s="12" t="s">
         <v>12</v>
@@ -13338,7 +13507,7 @@
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
       <c r="F152" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G152" s="12" t="s">
         <v>12</v>
@@ -13351,10 +13520,10 @@
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
       <c r="F153" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G153" s="15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13364,7 +13533,7 @@
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
       <c r="F154" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G154" s="12" t="s">
         <v>12</v>
@@ -13425,7 +13594,7 @@
         <v>10</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G159" s="12" t="s">
         <v>12</v>
@@ -13444,7 +13613,7 @@
       <c r="A161" s="13"/>
       <c r="B161" s="7"/>
       <c r="C161" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D161" s="10" t="s">
         <v>9</v>
@@ -13455,8 +13624,8 @@
       <c r="F161" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G161" s="14" t="s">
-        <v>131</v>
+      <c r="G161" s="17" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13466,7 +13635,7 @@
       <c r="D162" s="10"/>
       <c r="E162" s="5"/>
       <c r="F162" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G162" s="12" t="s">
         <v>12</v>
@@ -13479,7 +13648,7 @@
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
       <c r="F163" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G163" s="12" t="s">
         <v>12</v>
@@ -13492,7 +13661,7 @@
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
       <c r="F164" s="11" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G164" s="12" t="s">
         <v>12</v>
@@ -13505,7 +13674,7 @@
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
       <c r="F165" s="11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G165" s="12" t="s">
         <v>12</v>
@@ -13518,7 +13687,7 @@
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
       <c r="F166" s="11" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G166" s="12" t="s">
         <v>12</v>
@@ -13531,10 +13700,10 @@
       <c r="D167" s="5"/>
       <c r="E167" s="5"/>
       <c r="F167" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G167" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13562,17 +13731,17 @@
     <row r="170" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C170" s="7"/>
       <c r="D170" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F170" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G170" s="12" t="s">
         <v>12</v>
@@ -13585,7 +13754,7 @@
       <c r="D171" s="10"/>
       <c r="E171" s="5"/>
       <c r="F171" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G171" s="12" t="s">
         <v>12</v>
@@ -13596,11 +13765,11 @@
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E172" s="5"/>
       <c r="F172" s="11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G172" s="12" t="s">
         <v>12</v>
@@ -13613,7 +13782,7 @@
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
       <c r="F173" s="11" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G173" s="12" t="s">
         <v>12</v>
@@ -13633,7 +13802,7 @@
         <v>35</v>
       </c>
       <c r="G174" s="12" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13647,10 +13816,10 @@
     </row>
     <row r="176" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C176" s="7"/>
       <c r="D176" s="10" t="s">
@@ -13663,7 +13832,7 @@
         <v>24</v>
       </c>
       <c r="G176" s="17" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13673,10 +13842,10 @@
       <c r="D177" s="10"/>
       <c r="E177" s="5"/>
       <c r="F177" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G177" s="12" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13686,10 +13855,10 @@
       <c r="D178" s="10"/>
       <c r="E178" s="5"/>
       <c r="F178" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G178" s="12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13699,10 +13868,10 @@
       <c r="D179" s="10"/>
       <c r="E179" s="5"/>
       <c r="F179" s="16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G179" s="12" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13712,7 +13881,7 @@
       <c r="D180" s="10"/>
       <c r="E180" s="5"/>
       <c r="F180" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G180" s="12" t="s">
         <v>12</v>
@@ -13725,7 +13894,7 @@
       <c r="D181" s="10"/>
       <c r="E181" s="5"/>
       <c r="F181" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G181" s="12" t="s">
         <v>12</v>
@@ -13758,10 +13927,10 @@
       <c r="D184" s="5"/>
       <c r="E184" s="5"/>
       <c r="F184" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G184" s="12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13771,10 +13940,10 @@
       <c r="D185" s="5"/>
       <c r="E185" s="5"/>
       <c r="F185" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G185" s="15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13784,7 +13953,7 @@
       <c r="D186" s="5"/>
       <c r="E186" s="5"/>
       <c r="F186" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G186" s="12" t="s">
         <v>12</v>
@@ -13807,13 +13976,13 @@
         <v>33</v>
       </c>
       <c r="E188" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F188" s="10" t="s">
         <v>35</v>
       </c>
       <c r="G188" s="12" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13836,10 +14005,10 @@
         <v>10</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G190" s="12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13854,7 +14023,7 @@
     <row r="192" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C192" s="7"/>
       <c r="D192" s="10" t="s">
@@ -13867,7 +14036,7 @@
         <v>24</v>
       </c>
       <c r="G192" s="17" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -13877,7 +14046,7 @@
       <c r="D193" s="10"/>
       <c r="E193" s="5"/>
       <c r="F193" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G193" s="12" t="s">
         <v>12</v>
@@ -13903,7 +14072,7 @@
       <c r="D195" s="5"/>
       <c r="E195" s="5"/>
       <c r="F195" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G195" s="12" t="s">
         <v>12</v>
@@ -13916,7 +14085,7 @@
       <c r="D196" s="5"/>
       <c r="E196" s="5"/>
       <c r="F196" s="11" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G196" s="12" t="s">
         <v>12</v>
@@ -13929,7 +14098,7 @@
       <c r="D197" s="5"/>
       <c r="E197" s="5"/>
       <c r="F197" s="11" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G197" s="12" t="s">
         <v>12</v>
@@ -13949,13 +14118,13 @@
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
       <c r="D199" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E199" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F199" s="11" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G199" s="12" t="s">
         <v>12</v>
@@ -13968,7 +14137,7 @@
       <c r="D200" s="5"/>
       <c r="E200" s="5"/>
       <c r="F200" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G200" s="12" t="s">
         <v>12</v>
@@ -13997,7 +14166,7 @@
         <v>35</v>
       </c>
       <c r="G202" s="12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -14012,7 +14181,7 @@
     <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="13"/>
       <c r="B204" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C204" s="7"/>
       <c r="D204" s="10" t="s">
@@ -14024,8 +14193,8 @@
       <c r="F204" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G204" s="14" t="s">
-        <v>160</v>
+      <c r="G204" s="17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -14035,10 +14204,10 @@
       <c r="D205" s="10"/>
       <c r="E205" s="5"/>
       <c r="F205" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G205" s="12" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -14061,7 +14230,7 @@
       <c r="D207" s="5"/>
       <c r="E207" s="5"/>
       <c r="F207" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G207" s="12" t="s">
         <v>12</v>
@@ -14074,7 +14243,7 @@
       <c r="D208" s="5"/>
       <c r="E208" s="5"/>
       <c r="F208" s="11" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G208" s="12" t="s">
         <v>12</v>
@@ -14087,7 +14256,7 @@
       <c r="D209" s="5"/>
       <c r="E209" s="5"/>
       <c r="F209" s="11" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G209" s="12" t="s">
         <v>12</v>
@@ -14107,13 +14276,13 @@
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
       <c r="D211" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E211" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F211" s="11" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G211" s="12" t="s">
         <v>12</v>
@@ -14126,7 +14295,7 @@
       <c r="D212" s="5"/>
       <c r="E212" s="5"/>
       <c r="F212" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G212" s="12" t="s">
         <v>12</v>
@@ -14143,7 +14312,7 @@
     </row>
     <row r="214" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B214" s="7"/>
       <c r="C214" s="7"/>
@@ -14165,7 +14334,7 @@
       <c r="D215" s="10"/>
       <c r="E215" s="5"/>
       <c r="F215" s="16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G215" s="12" t="s">
         <v>12</v>
@@ -14178,7 +14347,7 @@
       <c r="D216" s="10"/>
       <c r="E216" s="10"/>
       <c r="F216" s="16" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G216" s="12" t="s">
         <v>12</v>
@@ -14204,7 +14373,7 @@
       <c r="D218" s="5"/>
       <c r="E218" s="5"/>
       <c r="F218" s="11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G218" s="12" t="s">
         <v>12</v>
@@ -14220,7 +14389,7 @@
         <v>19</v>
       </c>
       <c r="G219" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -14237,13 +14406,13 @@
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
       <c r="D221" s="10" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E221" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F221" s="11" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G221" s="12" t="s">
         <v>12</v>
@@ -14256,7 +14425,7 @@
       <c r="D222" s="5"/>
       <c r="E222" s="5"/>
       <c r="F222" s="11" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G222" s="12" t="s">
         <v>12</v>
@@ -14269,7 +14438,7 @@
       <c r="D223" s="5"/>
       <c r="E223" s="5"/>
       <c r="F223" s="11" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G223" s="12" t="s">
         <v>12</v>
@@ -14306,16 +14475,16 @@
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
       <c r="D226" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E226" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F226" s="11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G226" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -14325,7 +14494,7 @@
       <c r="D227" s="5"/>
       <c r="E227" s="5"/>
       <c r="F227" s="11" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="G227" s="12" t="s">
         <v>12</v>
@@ -14342,6 +14511,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:D108"/>
     <mergeCell ref="E129:E130"/>
     <mergeCell ref="G129:G130"/>
     <mergeCell ref="G110:G111"/>
@@ -14358,20 +14539,9 @@
     <mergeCell ref="A129:A130"/>
     <mergeCell ref="B129:B130"/>
     <mergeCell ref="C129:C130"/>
-    <mergeCell ref="D129:D130"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:D108"/>
-    <mergeCell ref="E107:E108"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>